<commit_message>
add detail week 4
</commit_message>
<xml_diff>
--- a/libraries/assets/grades/gradebook_percentage.xlsx
+++ b/libraries/assets/grades/gradebook_percentage.xlsx
@@ -1462,7 +1462,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.0</c:v>
@@ -1474,10 +1474,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1492,11 +1492,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2094650112"/>
-        <c:axId val="-2094646128"/>
+        <c:axId val="-2143070912"/>
+        <c:axId val="-2143067664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2094650112"/>
+        <c:axId val="-2143070912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1531,7 +1531,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2094646128"/>
+        <c:crossAx val="-2143067664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1541,7 +1541,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2094646128"/>
+        <c:axId val="-2143067664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +1615,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2094650112"/>
+        <c:crossAx val="-2143070912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1687,7 +1687,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Grades!A34:E49" spid="_x0000_s1086"/>
+                  <a14:cameraTool cellRange="Grades!A34:E49" spid="_x0000_s1088"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2236,7 +2236,7 @@
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2696,18 +2696,20 @@
       </c>
       <c r="U12" s="77"/>
       <c r="V12" s="77"/>
-      <c r="W12" s="77"/>
+      <c r="W12" s="77">
+        <v>0.97499999999999998</v>
+      </c>
       <c r="X12" s="77"/>
       <c r="Y12" s="77"/>
       <c r="Z12" s="77"/>
       <c r="AA12" s="77"/>
       <c r="AB12" s="71">
         <f t="shared" ref="AB12:AB25" si="0">IF(SUM(C12:AA12)=0,"",SUMPRODUCT(C12:AA12,$C$9:$AA$9))</f>
-        <v>140</v>
+        <v>286.25</v>
       </c>
       <c r="AC12" s="72">
         <f t="shared" ref="AC12:AC25" si="1">IF(SUM(C12:AA12)=0,"",$AC$9+AB12/(SUMIF(C12:AA12,"&lt;&gt;",$C$9:$AA$9)-SUMIF(C12:AA12,"=E",$C$9:$AA$9)))</f>
-        <v>1</v>
+        <v>0.98706896551724133</v>
       </c>
       <c r="AD12" s="73" t="str">
         <f>IF(AC12="","",INDEX(Grades!$B$12:$B$24,MATCH(AC12,Grades!$A$12:$A$24,1)))</f>
@@ -2760,22 +2762,24 @@
       </c>
       <c r="U13" s="77"/>
       <c r="V13" s="77"/>
-      <c r="W13" s="77"/>
+      <c r="W13" s="77">
+        <v>0.90500000000000003</v>
+      </c>
       <c r="X13" s="77"/>
       <c r="Y13" s="77"/>
       <c r="Z13" s="77"/>
       <c r="AA13" s="77"/>
       <c r="AB13" s="71">
         <f t="shared" si="0"/>
-        <v>137.5</v>
+        <v>273.25</v>
       </c>
       <c r="AC13" s="72">
         <f t="shared" si="1"/>
-        <v>0.9821428571428571</v>
+        <v>0.9422413793103448</v>
       </c>
       <c r="AD13" s="73" t="str">
         <f>IF(AC13="","",INDEX(Grades!$B$12:$B$24,MATCH(AC13,Grades!$A$12:$A$24,1)))</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="AF13" s="82" t="s">
         <v>86</v>
@@ -2824,18 +2828,20 @@
       </c>
       <c r="U14" s="77"/>
       <c r="V14" s="77"/>
-      <c r="W14" s="77"/>
+      <c r="W14" s="77">
+        <v>0.96</v>
+      </c>
       <c r="X14" s="77"/>
       <c r="Y14" s="77"/>
       <c r="Z14" s="77"/>
       <c r="AA14" s="77"/>
       <c r="AB14" s="71">
         <f t="shared" si="0"/>
-        <v>125.5</v>
+        <v>269.5</v>
       </c>
       <c r="AC14" s="72">
         <f t="shared" si="1"/>
-        <v>0.9653846153846154</v>
+        <v>0.96250000000000002</v>
       </c>
       <c r="AD14" s="73" t="str">
         <f>IF(AC14="","",INDEX(Grades!$B$12:$B$24,MATCH(AC14,Grades!$A$12:$A$24,1)))</f>
@@ -2888,18 +2894,20 @@
       </c>
       <c r="U15" s="77"/>
       <c r="V15" s="77"/>
-      <c r="W15" s="77"/>
+      <c r="W15" s="77">
+        <v>0.995</v>
+      </c>
       <c r="X15" s="77"/>
       <c r="Y15" s="77"/>
       <c r="Z15" s="77"/>
       <c r="AA15" s="77"/>
       <c r="AB15" s="71">
         <f t="shared" si="0"/>
-        <v>137.5</v>
+        <v>286.75</v>
       </c>
       <c r="AC15" s="72">
         <f t="shared" si="1"/>
-        <v>0.9821428571428571</v>
+        <v>0.98879310344827587</v>
       </c>
       <c r="AD15" s="73" t="str">
         <f>IF(AC15="","",INDEX(Grades!$B$12:$B$24,MATCH(AC15,Grades!$A$12:$A$24,1)))</f>
@@ -2952,18 +2960,20 @@
       </c>
       <c r="U16" s="77"/>
       <c r="V16" s="77"/>
-      <c r="W16" s="77"/>
+      <c r="W16" s="77">
+        <v>0.99</v>
+      </c>
       <c r="X16" s="77"/>
       <c r="Y16" s="77"/>
       <c r="Z16" s="77"/>
       <c r="AA16" s="77"/>
       <c r="AB16" s="71">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>288.5</v>
       </c>
       <c r="AC16" s="72">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.9948275862068966</v>
       </c>
       <c r="AD16" s="73" t="str">
         <f>IF(AC16="","",INDEX(Grades!$B$12:$B$24,MATCH(AC16,Grades!$A$12:$A$24,1)))</f>
@@ -3016,18 +3026,20 @@
       </c>
       <c r="U17" s="77"/>
       <c r="V17" s="77"/>
-      <c r="W17" s="77"/>
+      <c r="W17" s="77">
+        <v>0.94</v>
+      </c>
       <c r="X17" s="77"/>
       <c r="Y17" s="77"/>
       <c r="Z17" s="77"/>
       <c r="AA17" s="77"/>
       <c r="AB17" s="71">
         <f t="shared" si="0"/>
-        <v>137.5</v>
+        <v>278.5</v>
       </c>
       <c r="AC17" s="72">
         <f t="shared" si="1"/>
-        <v>0.9821428571428571</v>
+        <v>0.96034482758620687</v>
       </c>
       <c r="AD17" s="73" t="str">
         <f>IF(AC17="","",INDEX(Grades!$B$12:$B$24,MATCH(AC17,Grades!$A$12:$A$24,1)))</f>
@@ -3080,18 +3092,20 @@
       </c>
       <c r="U18" s="77"/>
       <c r="V18" s="77"/>
-      <c r="W18" s="77"/>
+      <c r="W18" s="77">
+        <v>0.96</v>
+      </c>
       <c r="X18" s="77"/>
       <c r="Y18" s="77"/>
       <c r="Z18" s="77"/>
       <c r="AA18" s="77"/>
       <c r="AB18" s="71">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>284</v>
       </c>
       <c r="AC18" s="72">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.97931034482758617</v>
       </c>
       <c r="AD18" s="73" t="str">
         <f>IF(AC18="","",INDEX(Grades!$B$12:$B$24,MATCH(AC18,Grades!$A$12:$A$24,1)))</f>
@@ -3144,18 +3158,20 @@
       </c>
       <c r="U19" s="77"/>
       <c r="V19" s="77"/>
-      <c r="W19" s="77"/>
+      <c r="W19" s="77">
+        <v>0.99</v>
+      </c>
       <c r="X19" s="77"/>
       <c r="Y19" s="77"/>
       <c r="Z19" s="77"/>
       <c r="AA19" s="77"/>
       <c r="AB19" s="71">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>288.5</v>
       </c>
       <c r="AC19" s="72">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.9948275862068966</v>
       </c>
       <c r="AD19" s="73" t="str">
         <f>IF(AC19="","",INDEX(Grades!$B$12:$B$24,MATCH(AC19,Grades!$A$12:$A$24,1)))</f>
@@ -3208,18 +3224,20 @@
       </c>
       <c r="U20" s="77"/>
       <c r="V20" s="77"/>
-      <c r="W20" s="77"/>
+      <c r="W20" s="77">
+        <v>0.97</v>
+      </c>
       <c r="X20" s="77"/>
       <c r="Y20" s="77"/>
       <c r="Z20" s="77"/>
       <c r="AA20" s="77"/>
       <c r="AB20" s="71">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>285.5</v>
       </c>
       <c r="AC20" s="72">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.98448275862068968</v>
       </c>
       <c r="AD20" s="73" t="str">
         <f>IF(AC20="","",INDEX(Grades!$B$12:$B$24,MATCH(AC20,Grades!$A$12:$A$24,1)))</f>
@@ -3272,18 +3290,20 @@
       </c>
       <c r="U21" s="77"/>
       <c r="V21" s="77"/>
-      <c r="W21" s="77"/>
+      <c r="W21" s="77">
+        <v>1.02</v>
+      </c>
       <c r="X21" s="77"/>
       <c r="Y21" s="77"/>
       <c r="Z21" s="77"/>
       <c r="AA21" s="77"/>
       <c r="AB21" s="71">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>293</v>
       </c>
       <c r="AC21" s="72">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.0103448275862068</v>
       </c>
       <c r="AD21" s="73" t="str">
         <f>IF(AC21="","",INDEX(Grades!$B$12:$B$24,MATCH(AC21,Grades!$A$12:$A$24,1)))</f>
@@ -3334,22 +3354,24 @@
       </c>
       <c r="U22" s="77"/>
       <c r="V22" s="77"/>
-      <c r="W22" s="77"/>
+      <c r="W22" s="77">
+        <v>0.69</v>
+      </c>
       <c r="X22" s="77"/>
       <c r="Y22" s="77"/>
       <c r="Z22" s="77"/>
       <c r="AA22" s="77"/>
       <c r="AB22" s="71">
         <f t="shared" si="0"/>
-        <v>136</v>
+        <v>239.5</v>
       </c>
       <c r="AC22" s="72">
         <f t="shared" si="1"/>
-        <v>0.97142857142857142</v>
+        <v>0.82586206896551728</v>
       </c>
       <c r="AD22" s="73" t="str">
         <f>IF(AC22="","",INDEX(Grades!$B$12:$B$24,MATCH(AC22,Grades!$A$12:$A$24,1)))</f>
-        <v>A+</v>
+        <v>B-</v>
       </c>
       <c r="AF22" s="84" t="s">
         <v>89</v>
@@ -3401,18 +3423,20 @@
       </c>
       <c r="U23" s="77"/>
       <c r="V23" s="77"/>
-      <c r="W23" s="77"/>
+      <c r="W23" s="77">
+        <v>1.01</v>
+      </c>
       <c r="X23" s="77"/>
       <c r="Y23" s="77"/>
       <c r="Z23" s="77"/>
       <c r="AA23" s="77"/>
       <c r="AB23" s="71">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>291.5</v>
       </c>
       <c r="AC23" s="72">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.0051724137931035</v>
       </c>
       <c r="AD23" s="73" t="str">
         <f>IF(AC23="","",INDEX(Grades!$B$12:$B$24,MATCH(AC23,Grades!$A$12:$A$24,1)))</f>
@@ -3462,18 +3486,20 @@
       </c>
       <c r="U24" s="77"/>
       <c r="V24" s="77"/>
-      <c r="W24" s="77"/>
+      <c r="W24" s="77">
+        <v>1.03</v>
+      </c>
       <c r="X24" s="77"/>
       <c r="Y24" s="77"/>
       <c r="Z24" s="77"/>
       <c r="AA24" s="77"/>
       <c r="AB24" s="71">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>294.5</v>
       </c>
       <c r="AC24" s="72">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.0155172413793103</v>
       </c>
       <c r="AD24" s="73" t="str">
         <f>IF(AC24="","",INDEX(Grades!$B$12:$B$24,MATCH(AC24,Grades!$A$12:$A$24,1)))</f>
@@ -3590,9 +3616,9 @@
         <f t="shared" ref="V26:AA26" si="4">IF(SUM(V12:V25)=0,"",AVERAGE(V12:V25))</f>
         <v/>
       </c>
-      <c r="W26" s="70" t="str">
+      <c r="W26" s="70">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0.95653846153846145</v>
       </c>
       <c r="X26" s="70" t="str">
         <f t="shared" si="4"/>
@@ -3615,7 +3641,7 @@
       </c>
       <c r="AC26" s="67">
         <f>AVERAGE(AC12:AC25)</f>
-        <v>0.99101859678782767</v>
+        <v>0.97317639257294419</v>
       </c>
       <c r="AD26" s="68" t="str">
         <f>IF(AC26="","",INDEX(Grades!$B$12:$B$24,MATCH(AC26,Grades!$A$12:$A$24,1)))</f>
@@ -3679,9 +3705,9 @@
         <f t="shared" ref="V27:AA27" si="6">IF(OR(V9=0,V26=""),"",MEDIAN(V12:V25))</f>
         <v/>
       </c>
-      <c r="W27" s="70" t="str">
+      <c r="W27" s="70">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0.97499999999999998</v>
       </c>
       <c r="X27" s="70" t="str">
         <f t="shared" si="6"/>
@@ -3704,7 +3730,7 @@
       </c>
       <c r="AC27" s="67">
         <f>MEDIAN(AC12:AC25)</f>
-        <v>1</v>
+        <v>0.98706896551724133</v>
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.15">
@@ -3764,9 +3790,9 @@
         <f t="shared" ref="V28:AA28" si="8">IF(OR(V9=0,V26=""),"",STDEV(V12:V25))</f>
         <v/>
       </c>
-      <c r="W28" s="70" t="str">
+      <c r="W28" s="70">
         <f t="shared" si="8"/>
-        <v/>
+        <v>8.6851996124264363E-2</v>
       </c>
       <c r="X28" s="70" t="str">
         <f t="shared" si="8"/>
@@ -3789,7 +3815,7 @@
       </c>
       <c r="AC28" s="67">
         <f>STDEV(AC12:AC25)</f>
-        <v>1.2657445727612258E-2</v>
+        <v>4.8883362637800833E-2</v>
       </c>
       <c r="AD28" s="31" t="s">
         <v>65</v>
@@ -4961,11 +4987,11 @@
       </c>
       <c r="C19" s="9">
         <f ca="1">COUNTIF(Gradebook!$AC$12:$AC$25,"&gt;="&amp;A19)-COUNTIF(Gradebook!$AC$12:$AC$25,"&gt;="&amp;OFFSET(A19,1,0,1,1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
@@ -5028,11 +5054,11 @@
       </c>
       <c r="C23" s="9">
         <f ca="1">COUNTIF(Gradebook!$AC$12:$AC$25,"&gt;="&amp;A23)-COUNTIF(Gradebook!$AC$12:$AC$25,"&gt;="&amp;OFFSET(A23,1,0,1,1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
@@ -5045,11 +5071,11 @@
       </c>
       <c r="C24" s="9">
         <f ca="1">COUNTIF(Gradebook!$AC$12:$AC$25,"&gt;="&amp;A24)-COUNTIF(Gradebook!$AC$12:$AC$25,"&gt;="&amp;OFFSET(A24,1,0,1,1))</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D24" s="29">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0.84615384615384615</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
@@ -5072,7 +5098,7 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="54">
         <f>Gradebook!$AC$26</f>
-        <v>0.99101859678782767</v>
+        <v>0.97317639257294419</v>
       </c>
       <c r="B28" s="55" t="str">
         <f>INDEX(B12:B24,MATCH(A28,A12:A24,1))</f>
@@ -5085,7 +5111,7 @@
       </c>
       <c r="B30" s="54">
         <f>Gradebook!AC27</f>
-        <v>1</v>
+        <v>0.98706896551724133</v>
       </c>
       <c r="C30" s="63" t="s">
         <v>56</v>
@@ -5097,7 +5123,7 @@
       </c>
       <c r="B31" s="54">
         <f>Gradebook!AC28</f>
-        <v>1.2657445727612258E-2</v>
+        <v>4.8883362637800833E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
@@ -5298,7 +5324,7 @@
       </c>
       <c r="B53" s="27">
         <f>PERCENTILE(Gradebook!$AC$12:$AC$25,A53)</f>
-        <v>1</v>
+        <v>1.0093103448275862</v>
       </c>
       <c r="C53" s="63" t="s">
         <v>62</v>
@@ -5312,7 +5338,7 @@
       </c>
       <c r="B54" s="27">
         <f>PERCENTILE(Gradebook!$AC$12:$AC$25,A54)</f>
-        <v>1</v>
+        <v>0.99362068965517247</v>
       </c>
       <c r="D54" s="28"/>
       <c r="E54" s="28"/>
@@ -5323,7 +5349,7 @@
       </c>
       <c r="B55" s="27">
         <f>PERCENTILE(Gradebook!$AC$12:$AC$25,A55)</f>
-        <v>0.98571428571428565</v>
+        <v>0.98034482758620689</v>
       </c>
       <c r="D55" s="28"/>
       <c r="E55" s="28"/>
@@ -5334,7 +5360,7 @@
       </c>
       <c r="B56" s="27">
         <f>PERCENTILE(Gradebook!$AC$12:$AC$25,A56)</f>
-        <v>0.97357142857142853</v>
+        <v>0.94586206896551717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
week 12, no entonation
</commit_message>
<xml_diff>
--- a/libraries/assets/grades/gradebook_percentage.xlsx
+++ b/libraries/assets/grades/gradebook_percentage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="28680" windowHeight="17460"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="32980" windowHeight="17740"/>
   </bookViews>
   <sheets>
     <sheet name="Gradebook" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="©" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Gradebook!$A$1:$AG$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Gradebook!$A$1:$AH$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Grades!$A$1:$J$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Names!$A$1:$H$109</definedName>
-    <definedName name="displayID">Gradebook!$AJ$24</definedName>
+    <definedName name="displayID">Gradebook!$AK$24</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Gradebook!$6:$11</definedName>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="155">
   <si>
     <t>Gradebook</t>
   </si>
@@ -514,6 +514,9 @@
   </si>
   <si>
     <t>Tarea 3</t>
+  </si>
+  <si>
+    <t>Pruebita 3</t>
   </si>
 </sst>
 </file>
@@ -959,7 +962,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -967,6 +970,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1211,13 +1215,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
@@ -1474,19 +1479,19 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1501,11 +1506,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2098713648"/>
-        <c:axId val="-2099713264"/>
+        <c:axId val="-2113217232"/>
+        <c:axId val="-2113209392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2098713648"/>
+        <c:axId val="-2113217232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1540,7 +1545,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2099713264"/>
+        <c:crossAx val="-2113209392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1550,7 +1555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2099713264"/>
+        <c:axId val="-2113209392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1624,7 +1629,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098713648"/>
+        <c:crossAx val="-2113217232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1679,13 +1684,13 @@
       <xdr:twoCellAnchor editAs="absolute">
         <xdr:from>
           <xdr:col>31</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
+          <xdr:colOff>165100</xdr:colOff>
           <xdr:row>25</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>34</xdr:col>
-          <xdr:colOff>1470611</xdr:colOff>
+          <xdr:col>35</xdr:col>
+          <xdr:colOff>937211</xdr:colOff>
           <xdr:row>40</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1696,7 +1701,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Grades!A34:E49" spid="_x0000_s1106"/>
+                  <a14:cameraTool cellRange="Grades!A34:E49" spid="_x0000_s1112"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1728,13 +1733,13 @@
   </mc:AlternateContent>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>1295400</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2242,28 +2247,28 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ28"/>
+  <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="3" customWidth="1"/>
-    <col min="3" max="19" width="7" style="3" customWidth="1"/>
-    <col min="20" max="22" width="8.33203125" style="3" customWidth="1"/>
-    <col min="23" max="30" width="7" style="3" customWidth="1"/>
-    <col min="31" max="31" width="8.5" style="3" customWidth="1"/>
-    <col min="32" max="32" width="7.5" style="3" customWidth="1"/>
-    <col min="33" max="33" width="8.83203125" style="3"/>
-    <col min="34" max="34" width="5.33203125" style="3" customWidth="1"/>
-    <col min="35" max="35" width="20.5" style="3" customWidth="1"/>
-    <col min="36" max="16384" width="8.83203125" style="3"/>
+    <col min="3" max="20" width="7" style="3" customWidth="1"/>
+    <col min="21" max="23" width="8.33203125" style="3" customWidth="1"/>
+    <col min="24" max="31" width="7" style="3" customWidth="1"/>
+    <col min="32" max="32" width="8.5" style="3" customWidth="1"/>
+    <col min="33" max="33" width="7.5" style="3" customWidth="1"/>
+    <col min="34" max="34" width="8.83203125" style="3"/>
+    <col min="35" max="35" width="5.33203125" style="3" customWidth="1"/>
+    <col min="36" max="36" width="20.5" style="3" customWidth="1"/>
+    <col min="37" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="88" t="s">
         <v>0</v>
       </c>
@@ -2298,19 +2303,20 @@
       <c r="AD1" s="7"/>
       <c r="AE1" s="7"/>
       <c r="AF1" s="7"/>
-      <c r="AI1" s="15"/>
-    </row>
-    <row r="2" spans="1:35" ht="14" x14ac:dyDescent="0.15">
+      <c r="AG1" s="7"/>
+      <c r="AJ1" s="15"/>
+    </row>
+    <row r="2" spans="1:36" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="12" t="s">
         <v>132</v>
       </c>
       <c r="F2" s="4"/>
-      <c r="AI2" s="46" t="s">
+      <c r="AJ2" s="46" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:36" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="11" t="s">
         <v>133</v>
@@ -2345,24 +2351,25 @@
       <c r="AD3" s="7"/>
       <c r="AE3" s="7"/>
       <c r="AF3" s="7"/>
-      <c r="AI3" s="22" t="s">
+      <c r="AG3" s="7"/>
+      <c r="AJ3" s="22" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:36" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" s="11" t="s">
         <v>134</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="AC4" s="80" t="s">
+      <c r="AD4" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="AD4" s="81" t="s">
+      <c r="AE4" s="81" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -2392,8 +2399,9 @@
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
-    </row>
-    <row r="6" spans="1:35" ht="14" x14ac:dyDescent="0.15">
+      <c r="AF5" s="4"/>
+    </row>
+    <row r="6" spans="1:36" ht="14" x14ac:dyDescent="0.15">
       <c r="B6" s="4"/>
       <c r="C6" s="65" t="s">
         <v>1</v>
@@ -2425,9 +2433,10 @@
       <c r="AB6" s="66"/>
       <c r="AC6" s="66"/>
       <c r="AD6" s="66"/>
-      <c r="AE6" s="4"/>
-    </row>
-    <row r="7" spans="1:35" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE6" s="66"/>
+      <c r="AF6" s="4"/>
+    </row>
+    <row r="7" spans="1:36" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="4"/>
       <c r="C7" s="94" t="s">
         <v>140</v>
@@ -2453,21 +2462,22 @@
       <c r="T7" s="96"/>
       <c r="U7" s="96"/>
       <c r="V7" s="96"/>
-      <c r="W7" s="96" t="s">
+      <c r="W7" s="96"/>
+      <c r="X7" s="96" t="s">
         <v>145</v>
       </c>
-      <c r="X7" s="96"/>
-      <c r="Y7" s="95"/>
-      <c r="Z7" s="95" t="s">
+      <c r="Y7" s="96"/>
+      <c r="Z7" s="95"/>
+      <c r="AA7" s="95" t="s">
         <v>141</v>
       </c>
-      <c r="AA7" s="95"/>
       <c r="AB7" s="95"/>
       <c r="AC7" s="95"/>
       <c r="AD7" s="95"/>
-      <c r="AE7" s="4"/>
-    </row>
-    <row r="8" spans="1:35" ht="67" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE7" s="95"/>
+      <c r="AF7" s="4"/>
+    </row>
+    <row r="8" spans="1:36" ht="67" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="91" t="s">
@@ -2522,41 +2532,44 @@
         <v>152</v>
       </c>
       <c r="T8" s="91" t="s">
+        <v>154</v>
+      </c>
+      <c r="U8" s="91" t="s">
         <v>150</v>
       </c>
-      <c r="U8" s="91" t="s">
+      <c r="V8" s="91" t="s">
         <v>151</v>
       </c>
-      <c r="V8" s="91" t="s">
+      <c r="W8" s="91" t="s">
         <v>153</v>
       </c>
-      <c r="W8" s="91" t="s">
+      <c r="X8" s="91" t="s">
         <v>143</v>
       </c>
-      <c r="X8" s="91" t="s">
+      <c r="Y8" s="91" t="s">
         <v>144</v>
       </c>
-      <c r="Y8" s="91" t="s">
+      <c r="Z8" s="91" t="s">
         <v>146</v>
       </c>
-      <c r="Z8" s="91" t="s">
+      <c r="AA8" s="91" t="s">
         <v>121</v>
       </c>
-      <c r="AA8" s="91" t="s">
+      <c r="AB8" s="91" t="s">
         <v>122</v>
       </c>
-      <c r="AB8" s="91" t="s">
+      <c r="AC8" s="91" t="s">
         <v>123</v>
       </c>
-      <c r="AC8" s="91" t="s">
+      <c r="AD8" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="AD8" s="79" t="s">
+      <c r="AE8" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="AE8" s="4"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="AF8" s="4"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="21" t="s">
         <v>35</v>
@@ -2613,7 +2626,7 @@
         <v>50</v>
       </c>
       <c r="T9" s="14">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="U9" s="14">
         <v>50</v>
@@ -2621,11 +2634,11 @@
       <c r="V9" s="14">
         <v>50</v>
       </c>
-      <c r="W9" s="14"/>
+      <c r="W9" s="14">
+        <v>50</v>
+      </c>
       <c r="X9" s="14"/>
-      <c r="Y9" s="14">
-        <v>150</v>
-      </c>
+      <c r="Y9" s="14"/>
       <c r="Z9" s="14">
         <v>150</v>
       </c>
@@ -2639,20 +2652,23 @@
         <v>150</v>
       </c>
       <c r="AD9" s="14">
+        <v>150</v>
+      </c>
+      <c r="AE9" s="14">
         <v>1000</v>
       </c>
-      <c r="AE9" s="34" t="s">
+      <c r="AF9" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="AF9" s="78">
+      <c r="AG9" s="78">
         <v>0</v>
       </c>
-      <c r="AI9" s="83" t="s">
+      <c r="AJ9" s="83" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="6" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:35" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:36" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="12" t="s">
         <v>51</v>
@@ -2685,20 +2701,21 @@
       <c r="AB11" s="20"/>
       <c r="AC11" s="20"/>
       <c r="AD11" s="20"/>
-      <c r="AE11" s="8" t="s">
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AF11" s="8" t="s">
+      <c r="AG11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AG11" s="8" t="s">
+      <c r="AH11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AI11" s="82" t="s">
+      <c r="AJ11" s="82" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A12" s="5">
         <f ca="1">OFFSET(A12,-1,0,1,1)+1</f>
         <v>1</v>
@@ -2737,8 +2754,12 @@
       <c r="L12" s="77">
         <v>1</v>
       </c>
-      <c r="M12" s="77"/>
-      <c r="N12" s="77"/>
+      <c r="M12" s="77">
+        <v>1</v>
+      </c>
+      <c r="N12" s="77">
+        <v>1</v>
+      </c>
       <c r="O12" s="77"/>
       <c r="P12" s="77"/>
       <c r="Q12" s="77"/>
@@ -2749,7 +2770,7 @@
         <v>0.91</v>
       </c>
       <c r="T12" s="77">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="U12" s="77">
         <v>1</v>
@@ -2757,39 +2778,44 @@
       <c r="V12" s="77">
         <v>1</v>
       </c>
-      <c r="W12" s="77" t="s">
+      <c r="W12" s="77">
+        <v>1</v>
+      </c>
+      <c r="X12" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X12" s="77"/>
       <c r="Y12" s="77"/>
-      <c r="Z12" s="77">
+      <c r="Z12" s="77"/>
+      <c r="AA12" s="77">
         <v>0.97499999999999998</v>
       </c>
-      <c r="AA12" s="77">
+      <c r="AB12" s="77">
         <v>0.94499999999999995</v>
       </c>
-      <c r="AB12" s="77"/>
-      <c r="AC12" s="77"/>
+      <c r="AC12" s="77">
+        <v>1.01</v>
+      </c>
       <c r="AD12" s="77"/>
-      <c r="AE12" s="71">
-        <f>IF(SUM(C12:AD12)=0,"",SUMPRODUCT(C12:AD12,$C$9:$AD$9))</f>
-        <v>633.5</v>
-      </c>
-      <c r="AF12" s="72">
-        <f>IF(SUM(C12:AD12)=0,"",$AF$9+AE12/(SUMIF(C12:AD12,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C12:AD12,"=E",$C$9:$AD$9)))</f>
-        <v>0.97461538461538466</v>
-      </c>
-      <c r="AG12" s="73" t="str">
-        <f>IF(AF12="","",INDEX(Grades!$B$12:$B$24,MATCH(AF12,Grades!$A$12:$A$24,1)))</f>
+      <c r="AE12" s="77"/>
+      <c r="AF12" s="71">
+        <f t="shared" ref="AF12:AF25" si="0">IF(SUM(C12:AE12)=0,"",SUMPRODUCT(C12:AE12,$C$9:$AE$9))</f>
+        <v>824</v>
+      </c>
+      <c r="AG12" s="72">
+        <f t="shared" ref="AG12:AG25" si="1">IF(SUM(C12:AE12)=0,"",$AG$9+AF12/(SUMIF(C12:AE12,"&lt;&gt;",$C$9:$AE$9)-SUMIF(C12:AE12,"=E",$C$9:$AE$9)))</f>
+        <v>0.98095238095238091</v>
+      </c>
+      <c r="AH12" s="73" t="str">
+        <f>IF(AG12="","",INDEX(Grades!$B$12:$B$24,MATCH(AG12,Grades!$A$12:$A$24,1)))</f>
         <v>A+</v>
       </c>
-      <c r="AI12" s="82" t="s">
+      <c r="AJ12" s="82" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A13" s="5">
-        <f t="shared" ref="A13:A24" ca="1" si="0">OFFSET(A13,-1,0,1,1)+1</f>
+        <f t="shared" ref="A13:A24" ca="1" si="2">OFFSET(A13,-1,0,1,1)+1</f>
         <v>2</v>
       </c>
       <c r="B13" s="76" t="str">
@@ -2826,8 +2852,12 @@
       <c r="L13" s="77">
         <v>0.85</v>
       </c>
-      <c r="M13" s="77"/>
-      <c r="N13" s="77"/>
+      <c r="M13" s="77">
+        <v>0.9</v>
+      </c>
+      <c r="N13" s="77">
+        <v>1</v>
+      </c>
       <c r="O13" s="77"/>
       <c r="P13" s="77"/>
       <c r="Q13" s="77"/>
@@ -2838,47 +2868,52 @@
         <v>0.25</v>
       </c>
       <c r="T13" s="77">
-        <v>1</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="U13" s="77">
         <v>1</v>
       </c>
       <c r="V13" s="77">
+        <v>1</v>
+      </c>
+      <c r="W13" s="77">
         <v>0</v>
       </c>
-      <c r="W13" s="77" t="s">
+      <c r="X13" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X13" s="77"/>
       <c r="Y13" s="77"/>
-      <c r="Z13" s="77">
+      <c r="Z13" s="77"/>
+      <c r="AA13" s="77">
         <v>0.90500000000000003</v>
       </c>
-      <c r="AA13" s="77">
+      <c r="AB13" s="77">
         <v>0.505</v>
       </c>
-      <c r="AB13" s="77"/>
-      <c r="AC13" s="77"/>
+      <c r="AC13" s="77">
+        <v>0.77500000000000002</v>
+      </c>
       <c r="AD13" s="77"/>
-      <c r="AE13" s="71">
-        <f>IF(SUM(C13:AD13)=0,"",SUMPRODUCT(C13:AD13,$C$9:$AD$9))</f>
-        <v>467</v>
-      </c>
-      <c r="AF13" s="72">
-        <f>IF(SUM(C13:AD13)=0,"",$AF$9+AE13/(SUMIF(C13:AD13,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C13:AD13,"=E",$C$9:$AD$9)))</f>
-        <v>0.71846153846153848</v>
-      </c>
-      <c r="AG13" s="73" t="str">
-        <f>IF(AF13="","",INDEX(Grades!$B$12:$B$24,MATCH(AF13,Grades!$A$12:$A$24,1)))</f>
+      <c r="AE13" s="77"/>
+      <c r="AF13" s="71">
+        <f t="shared" si="0"/>
+        <v>612.75</v>
+      </c>
+      <c r="AG13" s="72">
+        <f t="shared" si="1"/>
+        <v>0.72946428571428568</v>
+      </c>
+      <c r="AH13" s="73" t="str">
+        <f>IF(AG13="","",INDEX(Grades!$B$12:$B$24,MATCH(AG13,Grades!$A$12:$A$24,1)))</f>
         <v>C-</v>
       </c>
-      <c r="AI13" s="82" t="s">
+      <c r="AJ13" s="82" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A14" s="5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>3</v>
       </c>
       <c r="B14" s="76" t="str">
@@ -2915,8 +2950,12 @@
       <c r="L14" s="77">
         <v>1</v>
       </c>
-      <c r="M14" s="77"/>
-      <c r="N14" s="77"/>
+      <c r="M14" s="77">
+        <v>1</v>
+      </c>
+      <c r="N14" s="77">
+        <v>1</v>
+      </c>
       <c r="O14" s="77"/>
       <c r="P14" s="77"/>
       <c r="Q14" s="77"/>
@@ -2927,7 +2966,7 @@
         <v>1</v>
       </c>
       <c r="T14" s="77">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="U14" s="77">
         <v>1</v>
@@ -2935,39 +2974,44 @@
       <c r="V14" s="77">
         <v>1</v>
       </c>
-      <c r="W14" s="77" t="s">
+      <c r="W14" s="77">
+        <v>1</v>
+      </c>
+      <c r="X14" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X14" s="77"/>
       <c r="Y14" s="77"/>
-      <c r="Z14" s="77">
+      <c r="Z14" s="77"/>
+      <c r="AA14" s="77">
         <v>0.96</v>
       </c>
-      <c r="AA14" s="77">
+      <c r="AB14" s="77">
         <v>1.01</v>
       </c>
-      <c r="AB14" s="77"/>
-      <c r="AC14" s="77"/>
+      <c r="AC14" s="77">
+        <v>0.97</v>
+      </c>
       <c r="AD14" s="77"/>
-      <c r="AE14" s="71">
-        <f>IF(SUM(C14:AD14)=0,"",SUMPRODUCT(C14:AD14,$C$9:$AD$9))</f>
-        <v>631</v>
-      </c>
-      <c r="AF14" s="72">
-        <f>IF(SUM(C14:AD14)=0,"",$AF$9+AE14/(SUMIF(C14:AD14,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C14:AD14,"=E",$C$9:$AD$9)))</f>
-        <v>0.98593750000000002</v>
-      </c>
-      <c r="AG14" s="73" t="str">
-        <f>IF(AF14="","",INDEX(Grades!$B$12:$B$24,MATCH(AF14,Grades!$A$12:$A$24,1)))</f>
+      <c r="AE14" s="77"/>
+      <c r="AF14" s="71">
+        <f t="shared" si="0"/>
+        <v>812.5</v>
+      </c>
+      <c r="AG14" s="72">
+        <f t="shared" si="1"/>
+        <v>0.97891566265060237</v>
+      </c>
+      <c r="AH14" s="73" t="str">
+        <f>IF(AG14="","",INDEX(Grades!$B$12:$B$24,MATCH(AG14,Grades!$A$12:$A$24,1)))</f>
         <v>A+</v>
       </c>
-      <c r="AI14" s="82" t="s">
+      <c r="AJ14" s="82" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A15" s="5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
       <c r="B15" s="76" t="str">
@@ -3004,8 +3048,12 @@
       <c r="L15" s="77">
         <v>1</v>
       </c>
-      <c r="M15" s="77"/>
-      <c r="N15" s="77"/>
+      <c r="M15" s="77">
+        <v>1</v>
+      </c>
+      <c r="N15" s="77">
+        <v>0.85</v>
+      </c>
       <c r="O15" s="77"/>
       <c r="P15" s="77"/>
       <c r="Q15" s="77"/>
@@ -3016,47 +3064,52 @@
         <v>0.83</v>
       </c>
       <c r="T15" s="77">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="U15" s="77">
+        <v>1</v>
+      </c>
+      <c r="V15" s="77">
         <v>0</v>
       </c>
-      <c r="V15" s="77">
-        <v>1</v>
-      </c>
-      <c r="W15" s="77" t="s">
+      <c r="W15" s="77">
+        <v>1</v>
+      </c>
+      <c r="X15" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X15" s="77"/>
       <c r="Y15" s="77"/>
-      <c r="Z15" s="77">
+      <c r="Z15" s="77"/>
+      <c r="AA15" s="77">
         <v>0.995</v>
       </c>
-      <c r="AA15" s="77">
+      <c r="AB15" s="77">
         <v>0.97499999999999998</v>
       </c>
-      <c r="AB15" s="77"/>
-      <c r="AC15" s="77"/>
+      <c r="AC15" s="77">
+        <v>0.89500000000000002</v>
+      </c>
       <c r="AD15" s="77"/>
-      <c r="AE15" s="71">
-        <f>IF(SUM(C15:AD15)=0,"",SUMPRODUCT(C15:AD15,$C$9:$AD$9))</f>
-        <v>583</v>
-      </c>
-      <c r="AF15" s="72">
-        <f>IF(SUM(C15:AD15)=0,"",$AF$9+AE15/(SUMIF(C15:AD15,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C15:AD15,"=E",$C$9:$AD$9)))</f>
-        <v>0.89692307692307693</v>
-      </c>
-      <c r="AG15" s="73" t="str">
-        <f>IF(AF15="","",INDEX(Grades!$B$12:$B$24,MATCH(AF15,Grades!$A$12:$A$24,1)))</f>
+      <c r="AE15" s="77"/>
+      <c r="AF15" s="71">
+        <f t="shared" si="0"/>
+        <v>753.75</v>
+      </c>
+      <c r="AG15" s="72">
+        <f t="shared" si="1"/>
+        <v>0.8973214285714286</v>
+      </c>
+      <c r="AH15" s="73" t="str">
+        <f>IF(AG15="","",INDEX(Grades!$B$12:$B$24,MATCH(AG15,Grades!$A$12:$A$24,1)))</f>
         <v>B+</v>
       </c>
-      <c r="AI15" s="82" t="s">
+      <c r="AJ15" s="82" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A16" s="5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
       <c r="B16" s="76" t="str">
@@ -3093,8 +3146,12 @@
       <c r="L16" s="77">
         <v>1</v>
       </c>
-      <c r="M16" s="77"/>
-      <c r="N16" s="77"/>
+      <c r="M16" s="77">
+        <v>1</v>
+      </c>
+      <c r="N16" s="77">
+        <v>1</v>
+      </c>
       <c r="O16" s="77"/>
       <c r="P16" s="77"/>
       <c r="Q16" s="77"/>
@@ -3105,7 +3162,7 @@
         <v>0.83</v>
       </c>
       <c r="T16" s="77">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="U16" s="77">
         <v>1</v>
@@ -3113,39 +3170,44 @@
       <c r="V16" s="77">
         <v>1</v>
       </c>
-      <c r="W16" s="77" t="s">
+      <c r="W16" s="77">
+        <v>1</v>
+      </c>
+      <c r="X16" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X16" s="77"/>
       <c r="Y16" s="77"/>
-      <c r="Z16" s="77">
+      <c r="Z16" s="77"/>
+      <c r="AA16" s="77">
         <v>0.99</v>
       </c>
-      <c r="AA16" s="77">
+      <c r="AB16" s="77">
         <v>0.93500000000000005</v>
       </c>
-      <c r="AB16" s="77"/>
-      <c r="AC16" s="77"/>
+      <c r="AC16" s="77">
+        <v>0.93</v>
+      </c>
       <c r="AD16" s="77"/>
-      <c r="AE16" s="71">
-        <f>IF(SUM(C16:AD16)=0,"",SUMPRODUCT(C16:AD16,$C$9:$AD$9))</f>
-        <v>630.25</v>
-      </c>
-      <c r="AF16" s="72">
-        <f>IF(SUM(C16:AD16)=0,"",$AF$9+AE16/(SUMIF(C16:AD16,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C16:AD16,"=E",$C$9:$AD$9)))</f>
-        <v>0.96961538461538466</v>
-      </c>
-      <c r="AG16" s="73" t="str">
-        <f>IF(AF16="","",INDEX(Grades!$B$12:$B$24,MATCH(AF16,Grades!$A$12:$A$24,1)))</f>
+      <c r="AE16" s="77"/>
+      <c r="AF16" s="71">
+        <f t="shared" si="0"/>
+        <v>807.75</v>
+      </c>
+      <c r="AG16" s="72">
+        <f t="shared" si="1"/>
+        <v>0.96160714285714288</v>
+      </c>
+      <c r="AH16" s="73" t="str">
+        <f>IF(AG16="","",INDEX(Grades!$B$12:$B$24,MATCH(AG16,Grades!$A$12:$A$24,1)))</f>
         <v>A+</v>
       </c>
-      <c r="AI16" s="82" t="s">
+      <c r="AJ16" s="82" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A17" s="5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="B17" s="76" t="str">
@@ -3182,8 +3244,12 @@
       <c r="L17" s="77">
         <v>1</v>
       </c>
-      <c r="M17" s="77"/>
-      <c r="N17" s="77"/>
+      <c r="M17" s="77">
+        <v>0.9</v>
+      </c>
+      <c r="N17" s="77">
+        <v>1</v>
+      </c>
       <c r="O17" s="77"/>
       <c r="P17" s="77"/>
       <c r="Q17" s="77"/>
@@ -3194,7 +3260,7 @@
         <v>0.95</v>
       </c>
       <c r="T17" s="77">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="U17" s="77">
         <v>1</v>
@@ -3202,39 +3268,44 @@
       <c r="V17" s="77">
         <v>1</v>
       </c>
-      <c r="W17" s="77" t="s">
+      <c r="W17" s="77">
+        <v>1</v>
+      </c>
+      <c r="X17" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X17" s="77"/>
       <c r="Y17" s="77"/>
-      <c r="Z17" s="77">
-        <v>0.94</v>
-      </c>
+      <c r="Z17" s="77"/>
       <c r="AA17" s="77">
         <v>0.94</v>
       </c>
-      <c r="AB17" s="77"/>
-      <c r="AC17" s="77"/>
+      <c r="AB17" s="77">
+        <v>0.94</v>
+      </c>
+      <c r="AC17" s="77">
+        <v>0.82499999999999996</v>
+      </c>
       <c r="AD17" s="77"/>
-      <c r="AE17" s="71">
-        <f>IF(SUM(C17:AD17)=0,"",SUMPRODUCT(C17:AD17,$C$9:$AD$9))</f>
-        <v>627</v>
-      </c>
-      <c r="AF17" s="72">
-        <f>IF(SUM(C17:AD17)=0,"",$AF$9+AE17/(SUMIF(C17:AD17,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C17:AD17,"=E",$C$9:$AD$9)))</f>
-        <v>0.96461538461538465</v>
-      </c>
-      <c r="AG17" s="73" t="str">
-        <f>IF(AF17="","",INDEX(Grades!$B$12:$B$24,MATCH(AF17,Grades!$A$12:$A$24,1)))</f>
-        <v>A+</v>
-      </c>
-      <c r="AI17" s="82" t="s">
+      <c r="AE17" s="77"/>
+      <c r="AF17" s="71">
+        <f t="shared" si="0"/>
+        <v>784.75</v>
+      </c>
+      <c r="AG17" s="72">
+        <f t="shared" si="1"/>
+        <v>0.93422619047619049</v>
+      </c>
+      <c r="AH17" s="73" t="str">
+        <f>IF(AG17="","",INDEX(Grades!$B$12:$B$24,MATCH(AG17,Grades!$A$12:$A$24,1)))</f>
+        <v>A</v>
+      </c>
+      <c r="AJ17" s="82" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A18" s="5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>7</v>
       </c>
       <c r="B18" s="76" t="str">
@@ -3271,8 +3342,12 @@
       <c r="L18" s="77">
         <v>1</v>
       </c>
-      <c r="M18" s="77"/>
-      <c r="N18" s="77"/>
+      <c r="M18" s="77">
+        <v>1</v>
+      </c>
+      <c r="N18" s="77">
+        <v>0.85</v>
+      </c>
       <c r="O18" s="77"/>
       <c r="P18" s="77"/>
       <c r="Q18" s="77"/>
@@ -3283,47 +3358,52 @@
         <v>0.91</v>
       </c>
       <c r="T18" s="77">
-        <v>1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U18" s="77">
+        <v>1</v>
+      </c>
+      <c r="V18" s="77">
         <v>0.85</v>
       </c>
-      <c r="V18" s="77">
-        <v>1</v>
-      </c>
-      <c r="W18" s="77" t="s">
+      <c r="W18" s="77">
+        <v>1</v>
+      </c>
+      <c r="X18" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X18" s="77"/>
       <c r="Y18" s="77"/>
-      <c r="Z18" s="77">
+      <c r="Z18" s="77"/>
+      <c r="AA18" s="77">
         <v>0.96</v>
       </c>
-      <c r="AA18" s="77">
+      <c r="AB18" s="77">
         <v>0.96499999999999997</v>
       </c>
-      <c r="AB18" s="77"/>
-      <c r="AC18" s="77"/>
+      <c r="AC18" s="77">
+        <v>0.96</v>
+      </c>
       <c r="AD18" s="77"/>
-      <c r="AE18" s="71">
-        <f>IF(SUM(C18:AD18)=0,"",SUMPRODUCT(C18:AD18,$C$9:$AD$9))</f>
-        <v>626.75</v>
-      </c>
-      <c r="AF18" s="72">
-        <f>IF(SUM(C18:AD18)=0,"",$AF$9+AE18/(SUMIF(C18:AD18,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C18:AD18,"=E",$C$9:$AD$9)))</f>
-        <v>0.96423076923076922</v>
-      </c>
-      <c r="AG18" s="73" t="str">
-        <f>IF(AF18="","",INDEX(Grades!$B$12:$B$24,MATCH(AF18,Grades!$A$12:$A$24,1)))</f>
-        <v>A+</v>
-      </c>
-      <c r="AI18" s="82" t="s">
+      <c r="AE18" s="77"/>
+      <c r="AF18" s="71">
+        <f t="shared" si="0"/>
+        <v>800.25</v>
+      </c>
+      <c r="AG18" s="72">
+        <f t="shared" si="1"/>
+        <v>0.95267857142857137</v>
+      </c>
+      <c r="AH18" s="73" t="str">
+        <f>IF(AG18="","",INDEX(Grades!$B$12:$B$24,MATCH(AG18,Grades!$A$12:$A$24,1)))</f>
+        <v>A</v>
+      </c>
+      <c r="AJ18" s="82" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A19" s="5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>8</v>
       </c>
       <c r="B19" s="76" t="str">
@@ -3360,8 +3440,12 @@
       <c r="L19" s="77">
         <v>1</v>
       </c>
-      <c r="M19" s="77"/>
-      <c r="N19" s="77"/>
+      <c r="M19" s="77">
+        <v>1</v>
+      </c>
+      <c r="N19" s="77">
+        <v>0.95</v>
+      </c>
       <c r="O19" s="77"/>
       <c r="P19" s="77"/>
       <c r="Q19" s="77"/>
@@ -3372,7 +3456,7 @@
         <v>0.95</v>
       </c>
       <c r="T19" s="77">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="U19" s="77">
         <v>1</v>
@@ -3380,39 +3464,44 @@
       <c r="V19" s="77">
         <v>1</v>
       </c>
-      <c r="W19" s="77" t="s">
+      <c r="W19" s="77">
+        <v>1</v>
+      </c>
+      <c r="X19" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X19" s="77"/>
       <c r="Y19" s="77"/>
-      <c r="Z19" s="77">
+      <c r="Z19" s="77"/>
+      <c r="AA19" s="77">
         <v>0.99</v>
       </c>
-      <c r="AA19" s="77">
+      <c r="AB19" s="77">
         <v>0.94</v>
       </c>
-      <c r="AB19" s="77"/>
-      <c r="AC19" s="77"/>
+      <c r="AC19" s="77">
+        <v>0.91500000000000004</v>
+      </c>
       <c r="AD19" s="77"/>
-      <c r="AE19" s="71">
-        <f>IF(SUM(C19:AD19)=0,"",SUMPRODUCT(C19:AD19,$C$9:$AD$9))</f>
-        <v>637</v>
-      </c>
-      <c r="AF19" s="72">
-        <f>IF(SUM(C19:AD19)=0,"",$AF$9+AE19/(SUMIF(C19:AD19,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C19:AD19,"=E",$C$9:$AD$9)))</f>
-        <v>0.98</v>
-      </c>
-      <c r="AG19" s="73" t="str">
-        <f>IF(AF19="","",INDEX(Grades!$B$12:$B$24,MATCH(AF19,Grades!$A$12:$A$24,1)))</f>
+      <c r="AE19" s="77"/>
+      <c r="AF19" s="71">
+        <f t="shared" si="0"/>
+        <v>810.75</v>
+      </c>
+      <c r="AG19" s="72">
+        <f t="shared" si="1"/>
+        <v>0.96517857142857144</v>
+      </c>
+      <c r="AH19" s="73" t="str">
+        <f>IF(AG19="","",INDEX(Grades!$B$12:$B$24,MATCH(AG19,Grades!$A$12:$A$24,1)))</f>
         <v>A+</v>
       </c>
-      <c r="AI19" s="82" t="s">
+      <c r="AJ19" s="82" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A20" s="5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
       <c r="B20" s="76" t="str">
@@ -3449,8 +3538,12 @@
       <c r="L20" s="77">
         <v>1</v>
       </c>
-      <c r="M20" s="77"/>
-      <c r="N20" s="77"/>
+      <c r="M20" s="77">
+        <v>1</v>
+      </c>
+      <c r="N20" s="77">
+        <v>1</v>
+      </c>
       <c r="O20" s="77"/>
       <c r="P20" s="77"/>
       <c r="Q20" s="77"/>
@@ -3461,47 +3554,52 @@
         <v>0.41</v>
       </c>
       <c r="T20" s="77">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="U20" s="77">
+        <v>1</v>
+      </c>
+      <c r="V20" s="77">
         <v>0.85</v>
       </c>
-      <c r="V20" s="77">
-        <v>1</v>
-      </c>
-      <c r="W20" s="77" t="s">
+      <c r="W20" s="77">
+        <v>1</v>
+      </c>
+      <c r="X20" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X20" s="77"/>
       <c r="Y20" s="77"/>
-      <c r="Z20" s="77">
+      <c r="Z20" s="77"/>
+      <c r="AA20" s="77">
         <v>0.97</v>
       </c>
-      <c r="AA20" s="77">
+      <c r="AB20" s="77">
         <v>0.85</v>
       </c>
-      <c r="AB20" s="77"/>
-      <c r="AC20" s="77"/>
+      <c r="AC20" s="77">
+        <v>0.88500000000000001</v>
+      </c>
       <c r="AD20" s="77"/>
-      <c r="AE20" s="71">
-        <f>IF(SUM(C20:AD20)=0,"",SUMPRODUCT(C20:AD20,$C$9:$AD$9))</f>
-        <v>584.5</v>
-      </c>
-      <c r="AF20" s="72">
-        <f>IF(SUM(C20:AD20)=0,"",$AF$9+AE20/(SUMIF(C20:AD20,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C20:AD20,"=E",$C$9:$AD$9)))</f>
-        <v>0.89923076923076928</v>
-      </c>
-      <c r="AG20" s="73" t="str">
-        <f>IF(AF20="","",INDEX(Grades!$B$12:$B$24,MATCH(AF20,Grades!$A$12:$A$24,1)))</f>
+      <c r="AE20" s="77"/>
+      <c r="AF20" s="71">
+        <f t="shared" si="0"/>
+        <v>752.25</v>
+      </c>
+      <c r="AG20" s="72">
+        <f t="shared" si="1"/>
+        <v>0.89553571428571432</v>
+      </c>
+      <c r="AH20" s="73" t="str">
+        <f>IF(AG20="","",INDEX(Grades!$B$12:$B$24,MATCH(AG20,Grades!$A$12:$A$24,1)))</f>
         <v>B+</v>
       </c>
-      <c r="AI20" s="82" t="s">
+      <c r="AJ20" s="82" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A21" s="5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>10</v>
       </c>
       <c r="B21" s="76" t="str">
@@ -3538,8 +3636,12 @@
       <c r="L21" s="77">
         <v>1</v>
       </c>
-      <c r="M21" s="77"/>
-      <c r="N21" s="77"/>
+      <c r="M21" s="77">
+        <v>0.9</v>
+      </c>
+      <c r="N21" s="77">
+        <v>1</v>
+      </c>
       <c r="O21" s="77"/>
       <c r="P21" s="77"/>
       <c r="Q21" s="77"/>
@@ -3550,7 +3652,7 @@
         <v>0.83</v>
       </c>
       <c r="T21" s="77">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="U21" s="77">
         <v>1</v>
@@ -3558,37 +3660,42 @@
       <c r="V21" s="77">
         <v>1</v>
       </c>
-      <c r="W21" s="77" t="s">
+      <c r="W21" s="77">
+        <v>1</v>
+      </c>
+      <c r="X21" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X21" s="77"/>
       <c r="Y21" s="77"/>
-      <c r="Z21" s="77">
+      <c r="Z21" s="77"/>
+      <c r="AA21" s="77">
         <v>1.02</v>
       </c>
-      <c r="AA21" s="77">
+      <c r="AB21" s="77">
         <v>0.97</v>
       </c>
-      <c r="AB21" s="77"/>
-      <c r="AC21" s="77"/>
+      <c r="AC21" s="77">
+        <v>0.93</v>
+      </c>
       <c r="AD21" s="77"/>
-      <c r="AE21" s="71">
-        <f>IF(SUM(C21:AD21)=0,"",SUMPRODUCT(C21:AD21,$C$9:$AD$9))</f>
-        <v>640</v>
-      </c>
-      <c r="AF21" s="72">
-        <f>IF(SUM(C21:AD21)=0,"",$AF$9+AE21/(SUMIF(C21:AD21,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C21:AD21,"=E",$C$9:$AD$9)))</f>
-        <v>0.98461538461538467</v>
-      </c>
-      <c r="AG21" s="73" t="str">
-        <f>IF(AF21="","",INDEX(Grades!$B$12:$B$24,MATCH(AF21,Grades!$A$12:$A$24,1)))</f>
+      <c r="AE21" s="77"/>
+      <c r="AF21" s="71">
+        <f t="shared" si="0"/>
+        <v>816.5</v>
+      </c>
+      <c r="AG21" s="72">
+        <f t="shared" si="1"/>
+        <v>0.97202380952380951</v>
+      </c>
+      <c r="AH21" s="73" t="str">
+        <f>IF(AG21="","",INDEX(Grades!$B$12:$B$24,MATCH(AG21,Grades!$A$12:$A$24,1)))</f>
         <v>A+</v>
       </c>
-      <c r="AI21" s="82"/>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="AJ21" s="82"/>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A22" s="5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>11</v>
       </c>
       <c r="B22" s="76" t="str">
@@ -3625,8 +3732,12 @@
       <c r="L22" s="77">
         <v>1</v>
       </c>
-      <c r="M22" s="77"/>
-      <c r="N22" s="77"/>
+      <c r="M22" s="77">
+        <v>1</v>
+      </c>
+      <c r="N22" s="77">
+        <v>1</v>
+      </c>
       <c r="O22" s="77"/>
       <c r="P22" s="77"/>
       <c r="Q22" s="77"/>
@@ -3637,7 +3748,7 @@
         <v>0.875</v>
       </c>
       <c r="T22" s="77">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="U22" s="77">
         <v>1</v>
@@ -3645,42 +3756,47 @@
       <c r="V22" s="77">
         <v>1</v>
       </c>
-      <c r="W22" s="77" t="s">
+      <c r="W22" s="77">
+        <v>1</v>
+      </c>
+      <c r="X22" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X22" s="77"/>
       <c r="Y22" s="77"/>
-      <c r="Z22" s="77">
+      <c r="Z22" s="77"/>
+      <c r="AA22" s="77">
         <v>0.69</v>
       </c>
-      <c r="AA22" s="77">
+      <c r="AB22" s="77">
         <v>0.85499999999999998</v>
       </c>
-      <c r="AB22" s="77"/>
-      <c r="AC22" s="77"/>
+      <c r="AC22" s="77">
+        <v>0.78500000000000003</v>
+      </c>
       <c r="AD22" s="77"/>
-      <c r="AE22" s="71">
-        <f>IF(SUM(C22:AD22)=0,"",SUMPRODUCT(C22:AD22,$C$9:$AD$9))</f>
-        <v>571.5</v>
-      </c>
-      <c r="AF22" s="72">
-        <f>IF(SUM(C22:AD22)=0,"",$AF$9+AE22/(SUMIF(C22:AD22,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C22:AD22,"=E",$C$9:$AD$9)))</f>
-        <v>0.87923076923076926</v>
-      </c>
-      <c r="AG22" s="73" t="str">
-        <f>IF(AF22="","",INDEX(Grades!$B$12:$B$24,MATCH(AF22,Grades!$A$12:$A$24,1)))</f>
-        <v>B+</v>
-      </c>
-      <c r="AI22" s="84" t="s">
+      <c r="AE22" s="77"/>
+      <c r="AF22" s="71">
+        <f t="shared" si="0"/>
+        <v>722.25</v>
+      </c>
+      <c r="AG22" s="72">
+        <f t="shared" si="1"/>
+        <v>0.85982142857142863</v>
+      </c>
+      <c r="AH22" s="73" t="str">
+        <f>IF(AG22="","",INDEX(Grades!$B$12:$B$24,MATCH(AG22,Grades!$A$12:$A$24,1)))</f>
+        <v>B</v>
+      </c>
+      <c r="AJ22" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="AJ22" s="85" t="s">
+      <c r="AK22" s="85" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A23" s="5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>12</v>
       </c>
       <c r="B23" s="76" t="str">
@@ -3717,8 +3833,12 @@
       <c r="L23" s="77">
         <v>1</v>
       </c>
-      <c r="M23" s="77"/>
-      <c r="N23" s="77"/>
+      <c r="M23" s="77">
+        <v>1</v>
+      </c>
+      <c r="N23" s="77">
+        <v>0.85</v>
+      </c>
       <c r="O23" s="77"/>
       <c r="P23" s="77"/>
       <c r="Q23" s="77"/>
@@ -3729,7 +3849,7 @@
         <v>0.83</v>
       </c>
       <c r="T23" s="77">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="U23" s="77">
         <v>1</v>
@@ -3737,36 +3857,41 @@
       <c r="V23" s="77">
         <v>1</v>
       </c>
-      <c r="W23" s="77" t="s">
+      <c r="W23" s="77">
+        <v>1</v>
+      </c>
+      <c r="X23" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X23" s="77"/>
       <c r="Y23" s="77"/>
-      <c r="Z23" s="77">
+      <c r="Z23" s="77"/>
+      <c r="AA23" s="77">
         <v>1.01</v>
       </c>
-      <c r="AA23" s="77">
+      <c r="AB23" s="77">
         <v>0.98499999999999999</v>
       </c>
-      <c r="AB23" s="77"/>
-      <c r="AC23" s="77"/>
+      <c r="AC23" s="77">
+        <v>0.97499999999999998</v>
+      </c>
       <c r="AD23" s="77"/>
-      <c r="AE23" s="71">
-        <f>IF(SUM(C23:AD23)=0,"",SUMPRODUCT(C23:AD23,$C$9:$AD$9))</f>
-        <v>640.75</v>
-      </c>
-      <c r="AF23" s="72">
-        <f>IF(SUM(C23:AD23)=0,"",$AF$9+AE23/(SUMIF(C23:AD23,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C23:AD23,"=E",$C$9:$AD$9)))</f>
-        <v>0.98576923076923073</v>
-      </c>
-      <c r="AG23" s="73" t="str">
-        <f>IF(AF23="","",INDEX(Grades!$B$12:$B$24,MATCH(AF23,Grades!$A$12:$A$24,1)))</f>
+      <c r="AE23" s="77"/>
+      <c r="AF23" s="71">
+        <f t="shared" si="0"/>
+        <v>823.5</v>
+      </c>
+      <c r="AG23" s="72">
+        <f t="shared" si="1"/>
+        <v>0.98035714285714282</v>
+      </c>
+      <c r="AH23" s="73" t="str">
+        <f>IF(AG23="","",INDEX(Grades!$B$12:$B$24,MATCH(AG23,Grades!$A$12:$A$24,1)))</f>
         <v>A+</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A24" s="5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>13</v>
       </c>
       <c r="B24" s="76" t="str">
@@ -3803,8 +3928,12 @@
       <c r="L24" s="77">
         <v>1</v>
       </c>
-      <c r="M24" s="77"/>
-      <c r="N24" s="77"/>
+      <c r="M24" s="77">
+        <v>1</v>
+      </c>
+      <c r="N24" s="77">
+        <v>1</v>
+      </c>
       <c r="O24" s="77"/>
       <c r="P24" s="77"/>
       <c r="Q24" s="77"/>
@@ -3815,7 +3944,7 @@
         <v>1</v>
       </c>
       <c r="T24" s="77">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="U24" s="77">
         <v>1</v>
@@ -3823,41 +3952,46 @@
       <c r="V24" s="77">
         <v>1</v>
       </c>
-      <c r="W24" s="77" t="s">
+      <c r="W24" s="77">
+        <v>1</v>
+      </c>
+      <c r="X24" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="X24" s="77"/>
       <c r="Y24" s="77"/>
-      <c r="Z24" s="77">
+      <c r="Z24" s="77"/>
+      <c r="AA24" s="77">
         <v>1.03</v>
       </c>
-      <c r="AA24" s="77">
+      <c r="AB24" s="77">
         <v>1.01</v>
       </c>
-      <c r="AB24" s="77"/>
-      <c r="AC24" s="77"/>
+      <c r="AC24" s="77">
+        <v>1.03</v>
+      </c>
       <c r="AD24" s="77"/>
-      <c r="AE24" s="71">
-        <f>IF(SUM(C24:AD24)=0,"",SUMPRODUCT(C24:AD24,$C$9:$AD$9))</f>
-        <v>656</v>
-      </c>
-      <c r="AF24" s="72">
-        <f>IF(SUM(C24:AD24)=0,"",$AF$9+AE24/(SUMIF(C24:AD24,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C24:AD24,"=E",$C$9:$AD$9)))</f>
-        <v>1.0092307692307692</v>
-      </c>
-      <c r="AG24" s="73" t="str">
-        <f>IF(AF24="","",INDEX(Grades!$B$12:$B$24,MATCH(AF24,Grades!$A$12:$A$24,1)))</f>
+      <c r="AE24" s="77"/>
+      <c r="AF24" s="71">
+        <f t="shared" si="0"/>
+        <v>849.5</v>
+      </c>
+      <c r="AG24" s="72">
+        <f t="shared" si="1"/>
+        <v>1.0113095238095238</v>
+      </c>
+      <c r="AH24" s="73" t="str">
+        <f>IF(AG24="","",INDEX(Grades!$B$12:$B$24,MATCH(AG24,Grades!$A$12:$A$24,1)))</f>
         <v>A+</v>
       </c>
-      <c r="AI24" s="86" t="s">
+      <c r="AJ24" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="AJ24" s="87" t="b">
-        <f>AJ22="Yes"</f>
+      <c r="AK24" s="87" t="b">
+        <f>AK22="Yes"</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A25" s="31" t="s">
         <v>65</v>
       </c>
@@ -3890,65 +4024,75 @@
       <c r="AB25" s="75"/>
       <c r="AC25" s="75"/>
       <c r="AD25" s="75"/>
-      <c r="AE25" s="71" t="str">
-        <f>IF(SUM(C25:AD25)=0,"",SUMPRODUCT(C25:AD25,$C$9:$AD$9))</f>
+      <c r="AE25" s="75"/>
+      <c r="AF25" s="71" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AF25" s="72" t="str">
-        <f>IF(SUM(C25:AD25)=0,"",$AF$9+AE25/(SUMIF(C25:AD25,"&lt;&gt;",$C$9:$AD$9)-SUMIF(C25:AD25,"=E",$C$9:$AD$9)))</f>
+      <c r="AG25" s="72" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AG25" s="73" t="str">
-        <f>IF(AF25="","",INDEX(Grades!$B$12:$B$24,MATCH(AF25,Grades!$A$12:$A$24,1)))</f>
+      <c r="AH25" s="73" t="str">
+        <f>IF(AG25="","",INDEX(Grades!$B$12:$B$24,MATCH(AG25,Grades!$A$12:$A$24,1)))</f>
         <v/>
       </c>
-      <c r="AI25" s="82" t="s">
+      <c r="AJ25" s="82" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B26" s="69" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="70">
-        <f t="shared" ref="C26:K26" si="1">IF(SUM(C12:C25)=0,"",AVERAGE(C12:C25))</f>
+        <f t="shared" ref="C26:K26" si="3">IF(SUM(C12:C25)=0,"",AVERAGE(C12:C25))</f>
         <v>1</v>
       </c>
       <c r="D26" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.99615384615384606</v>
       </c>
       <c r="E26" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F26" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.97692307692307689</v>
       </c>
       <c r="G26" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.97692307692307689</v>
       </c>
       <c r="H26" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.98846153846153839</v>
       </c>
       <c r="I26" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.98846153846153839</v>
       </c>
       <c r="J26" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K26" s="70">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L26" s="70"/>
-      <c r="M26" s="70"/>
-      <c r="N26" s="70"/>
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L26" s="70">
+        <f t="shared" ref="L26:N26" si="4">IF(SUM(L12:L25)=0,"",AVERAGE(L12:L25))</f>
+        <v>0.98846153846153839</v>
+      </c>
+      <c r="M26" s="70">
+        <f t="shared" si="4"/>
+        <v>0.97692307692307701</v>
+      </c>
+      <c r="N26" s="70">
+        <f t="shared" si="4"/>
+        <v>0.96153846153846145</v>
+      </c>
       <c r="O26" s="70"/>
       <c r="P26" s="70"/>
       <c r="Q26" s="70" t="str">
@@ -3963,90 +4107,112 @@
         <f>IF(SUM(S12:S25)=0,"",AVERAGE(S12:S25))</f>
         <v>0.81346153846153857</v>
       </c>
-      <c r="T26" s="70"/>
-      <c r="U26" s="70"/>
-      <c r="V26" s="70"/>
-      <c r="W26" s="70"/>
+      <c r="T26" s="70">
+        <f>IF(SUM(T12:T25)=0,"",AVERAGE(T12:T25))</f>
+        <v>0.79807692307692313</v>
+      </c>
+      <c r="U26" s="70">
+        <f>IF(SUM(U12:U25)=0,"",AVERAGE(U12:U25))</f>
+        <v>1</v>
+      </c>
+      <c r="V26" s="70">
+        <f>IF(SUM(V12:V25)=0,"",AVERAGE(V12:V25))</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="W26" s="70">
+        <f>IF(SUM(W12:W25)=0,"",AVERAGE(W12:W25))</f>
+        <v>0.92307692307692313</v>
+      </c>
       <c r="X26" s="70"/>
-      <c r="Y26" s="70" t="str">
-        <f t="shared" ref="Y26:AD26" si="2">IF(SUM(Y12:Y25)=0,"",AVERAGE(Y12:Y25))</f>
+      <c r="Y26" s="70"/>
+      <c r="Z26" s="70" t="str">
+        <f t="shared" ref="Z26:AE26" si="5">IF(SUM(Z12:Z25)=0,"",AVERAGE(Z12:Z25))</f>
         <v/>
       </c>
-      <c r="Z26" s="70">
-        <f t="shared" si="2"/>
+      <c r="AA26" s="70">
+        <f t="shared" si="5"/>
         <v>0.95653846153846145</v>
       </c>
-      <c r="AA26" s="70">
-        <f t="shared" si="2"/>
+      <c r="AB26" s="70">
+        <f t="shared" si="5"/>
         <v>0.91423076923076918</v>
       </c>
-      <c r="AB26" s="70" t="str">
-        <f t="shared" si="2"/>
+      <c r="AC26" s="70">
+        <f t="shared" si="5"/>
+        <v>0.91423076923076918</v>
+      </c>
+      <c r="AD26" s="70" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="AC26" s="70" t="str">
-        <f t="shared" si="2"/>
+      <c r="AE26" s="70" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="AD26" s="70" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AE26" s="19" t="s">
+      <c r="AF26" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="AF26" s="67">
-        <f>AVERAGE(AF12:AF25)</f>
-        <v>0.93942122781065085</v>
-      </c>
-      <c r="AG26" s="68" t="str">
-        <f>IF(AF26="","",INDEX(Grades!$B$12:$B$24,MATCH(AF26,Grades!$A$12:$A$24,1)))</f>
+      <c r="AG26" s="67">
+        <f>AVERAGE(AG12:AG25)</f>
+        <v>0.93226091177898418</v>
+      </c>
+      <c r="AH26" s="68" t="str">
+        <f>IF(AG26="","",INDEX(Grades!$B$12:$B$24,MATCH(AG26,Grades!$A$12:$A$24,1)))</f>
         <v>A</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B27" s="69" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="70">
-        <f t="shared" ref="C27:K27" si="3">IF(OR(C9=0,C26=""),"",MEDIAN(C12:C25))</f>
+        <f t="shared" ref="C27:K27" si="6">IF(OR(C9=0,C26=""),"",MEDIAN(C12:C25))</f>
         <v>1</v>
       </c>
       <c r="D27" s="70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E27" s="70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="F27" s="70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G27" s="70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H27" s="70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I27" s="70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J27" s="70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K27" s="70">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L27" s="70"/>
-      <c r="M27" s="70"/>
-      <c r="N27" s="70"/>
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L27" s="70">
+        <f t="shared" ref="L27:N27" si="7">IF(OR(L9=0,L26=""),"",MEDIAN(L12:L25))</f>
+        <v>1</v>
+      </c>
+      <c r="M27" s="70">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N27" s="70">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
       <c r="O27" s="70"/>
       <c r="P27" s="70"/>
       <c r="Q27" s="70" t="str">
@@ -4054,93 +4220,115 @@
         <v/>
       </c>
       <c r="R27" s="70">
-        <f t="shared" ref="R27:S27" si="4">IF(OR(R9=0,R26=""),"",MEDIAN(R12:R25))</f>
+        <f t="shared" ref="R27:S27" si="8">IF(OR(R9=0,R26=""),"",MEDIAN(R12:R25))</f>
         <v>1</v>
       </c>
       <c r="S27" s="70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.875</v>
       </c>
-      <c r="T27" s="70"/>
-      <c r="U27" s="70"/>
-      <c r="V27" s="70"/>
-      <c r="W27" s="70"/>
+      <c r="T27" s="70">
+        <f t="shared" ref="T27:W27" si="9">IF(OR(T9=0,T26=""),"",MEDIAN(T12:T25))</f>
+        <v>0.85</v>
+      </c>
+      <c r="U27" s="70">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="V27" s="70">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="W27" s="70">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
       <c r="X27" s="70"/>
-      <c r="Y27" s="70" t="str">
-        <f t="shared" ref="Y27:AD27" si="5">IF(OR(Y9=0,Y26=""),"",MEDIAN(Y12:Y25))</f>
+      <c r="Y27" s="70"/>
+      <c r="Z27" s="70" t="str">
+        <f t="shared" ref="Z27:AE27" si="10">IF(OR(Z9=0,Z26=""),"",MEDIAN(Z12:Z25))</f>
         <v/>
       </c>
-      <c r="Z27" s="70">
-        <f t="shared" si="5"/>
+      <c r="AA27" s="70">
+        <f t="shared" si="10"/>
         <v>0.97499999999999998</v>
       </c>
-      <c r="AA27" s="70">
-        <f t="shared" si="5"/>
+      <c r="AB27" s="70">
+        <f t="shared" si="10"/>
         <v>0.94499999999999995</v>
       </c>
-      <c r="AB27" s="70" t="str">
-        <f t="shared" si="5"/>
+      <c r="AC27" s="70">
+        <f t="shared" si="10"/>
+        <v>0.93</v>
+      </c>
+      <c r="AD27" s="70" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AC27" s="70" t="str">
-        <f t="shared" si="5"/>
+      <c r="AE27" s="70" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AD27" s="70" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AE27" s="19" t="s">
+      <c r="AF27" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="AF27" s="67">
-        <f>MEDIAN(AF12:AF25)</f>
-        <v>0.96961538461538466</v>
-      </c>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="AG27" s="67">
+        <f>MEDIAN(AG12:AG25)</f>
+        <v>0.96160714285714288</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B28" s="69" t="s">
         <v>50</v>
       </c>
       <c r="C28" s="70">
-        <f t="shared" ref="C28:K28" si="6">IF(OR(C9=0,C26=""),"",STDEV(C12:C25))</f>
+        <f t="shared" ref="C28:K28" si="11">IF(OR(C9=0,C26=""),"",STDEV(C12:C25))</f>
         <v>0</v>
       </c>
       <c r="D28" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1.3867504905630743E-2</v>
       </c>
       <c r="E28" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F28" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5.6330071214910814E-2</v>
       </c>
       <c r="G28" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>8.3205029433784355E-2</v>
       </c>
       <c r="H28" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4.1602514716892199E-2</v>
       </c>
       <c r="I28" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4.1602514716892199E-2</v>
       </c>
       <c r="J28" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K28" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="L28" s="70"/>
-      <c r="M28" s="70"/>
-      <c r="N28" s="70"/>
+      <c r="L28" s="70">
+        <f t="shared" ref="L28:N28" si="12">IF(OR(L9=0,L26=""),"",STDEV(L12:L25))</f>
+        <v>4.1602514716892199E-2</v>
+      </c>
+      <c r="M28" s="70">
+        <f t="shared" si="12"/>
+        <v>4.3852900965351452E-2</v>
+      </c>
+      <c r="N28" s="70">
+        <f t="shared" si="12"/>
+        <v>6.5044363558799098E-2</v>
+      </c>
       <c r="O28" s="70"/>
       <c r="P28" s="70"/>
       <c r="Q28" s="70" t="str">
@@ -4148,62 +4336,75 @@
         <v/>
       </c>
       <c r="R28" s="70">
-        <f t="shared" ref="R28:S28" si="7">IF(OR(R9=0,R26=""),"",STDEV(R12:R25))</f>
+        <f t="shared" ref="R28:S28" si="13">IF(OR(R9=0,R26=""),"",STDEV(R12:R25))</f>
         <v>2.5318484177091691E-2</v>
       </c>
       <c r="S28" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.22558613114307899</v>
       </c>
-      <c r="T28" s="70"/>
-      <c r="U28" s="70"/>
-      <c r="V28" s="70"/>
-      <c r="W28" s="70"/>
+      <c r="T28" s="70">
+        <f t="shared" ref="T28:W28" si="14">IF(OR(T9=0,T26=""),"",STDEV(T12:T25))</f>
+        <v>0.14522308215205881</v>
+      </c>
+      <c r="U28" s="70">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="V28" s="70">
+        <f t="shared" si="14"/>
+        <v>0.27613402542968168</v>
+      </c>
+      <c r="W28" s="70">
+        <f t="shared" si="14"/>
+        <v>0.27735009811261457</v>
+      </c>
       <c r="X28" s="70"/>
-      <c r="Y28" s="70" t="str">
-        <f t="shared" ref="Y28:AD28" si="8">IF(OR(Y9=0,Y26=""),"",STDEV(Y12:Y25))</f>
+      <c r="Y28" s="70"/>
+      <c r="Z28" s="70" t="str">
+        <f t="shared" ref="Z28:AE28" si="15">IF(OR(Z9=0,Z26=""),"",STDEV(Z12:Z25))</f>
         <v/>
       </c>
-      <c r="Z28" s="70">
-        <f t="shared" si="8"/>
+      <c r="AA28" s="70">
+        <f t="shared" si="15"/>
         <v>8.6851996124264363E-2</v>
       </c>
-      <c r="AA28" s="70">
-        <f t="shared" si="8"/>
+      <c r="AB28" s="70">
+        <f t="shared" si="15"/>
         <v>0.13245826628675214</v>
       </c>
-      <c r="AB28" s="70" t="str">
-        <f t="shared" si="8"/>
+      <c r="AC28" s="70">
+        <f t="shared" si="15"/>
+        <v>8.0230037855898925E-2</v>
+      </c>
+      <c r="AD28" s="70" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AC28" s="70" t="str">
-        <f t="shared" si="8"/>
+      <c r="AE28" s="70" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AD28" s="70" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="AE28" s="19" t="s">
+      <c r="AF28" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="AF28" s="67">
-        <f>STDEV(AF12:AF25)</f>
-        <v>7.7536248331331728E-2</v>
-      </c>
-      <c r="AG28" s="31" t="s">
+      <c r="AG28" s="67">
+        <f>STDEV(AG12:AG25)</f>
+        <v>7.4161714136325566E-2</v>
+      </c>
+      <c r="AH28" s="31" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK22">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="AI3" r:id="rId1"/>
+    <hyperlink ref="AJ3" r:id="rId1"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>
@@ -5241,7 +5442,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A12)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A12,1,0,1,1))</f>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A12)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A12,1,0,1,1))</f>
         <v>0</v>
       </c>
       <c r="D12" s="16">
@@ -5257,7 +5458,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A13)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A13,1,0,1,1))</f>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A13)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A13,1,0,1,1))</f>
         <v>0</v>
       </c>
       <c r="D13" s="16">
@@ -5274,7 +5475,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A14)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A14,1,0,1,1))</f>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A14)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A14,1,0,1,1))</f>
         <v>0</v>
       </c>
       <c r="D14" s="16">
@@ -5291,7 +5492,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A15)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A15,1,0,1,1))</f>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A15)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A15,1,0,1,1))</f>
         <v>0</v>
       </c>
       <c r="D15" s="16">
@@ -5307,7 +5508,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A16)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A16,1,0,1,1))</f>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A16)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A16,1,0,1,1))</f>
         <v>1</v>
       </c>
       <c r="D16" s="16">
@@ -5327,7 +5528,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A17)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A17,1,0,1,1))</f>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A17)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A17,1,0,1,1))</f>
         <v>0</v>
       </c>
       <c r="D17" s="16">
@@ -5344,7 +5545,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A18)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A18,1,0,1,1))</f>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A18)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A18,1,0,1,1))</f>
         <v>0</v>
       </c>
       <c r="D18" s="16">
@@ -5360,7 +5561,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A19)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A19,1,0,1,1))</f>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A19)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A19,1,0,1,1))</f>
         <v>0</v>
       </c>
       <c r="D19" s="16">
@@ -5377,12 +5578,12 @@
         <v>10</v>
       </c>
       <c r="C20" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A20)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A20,1,0,1,1))</f>
-        <v>0</v>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A20)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A20,1,0,1,1))</f>
+        <v>1</v>
       </c>
       <c r="D20" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
@@ -5394,12 +5595,12 @@
         <v>9</v>
       </c>
       <c r="C21" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A21)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A21,1,0,1,1))</f>
-        <v>3</v>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A21)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A21,1,0,1,1))</f>
+        <v>2</v>
       </c>
       <c r="D21" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23076923076923078</v>
+        <v>0.15384615384615385</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
@@ -5410,7 +5611,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A22)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A22,1,0,1,1))</f>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A22)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A22,1,0,1,1))</f>
         <v>0</v>
       </c>
       <c r="D22" s="16">
@@ -5427,12 +5628,12 @@
         <v>7</v>
       </c>
       <c r="C23" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A23)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A23,1,0,1,1))</f>
-        <v>0</v>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A23)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A23,1,0,1,1))</f>
+        <v>2</v>
       </c>
       <c r="D23" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.15384615384615385</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
@@ -5444,12 +5645,12 @@
         <v>6</v>
       </c>
       <c r="C24" s="9">
-        <f ca="1">COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;A24)-COUNTIF(Gradebook!$AF$12:$AF$25,"&gt;="&amp;OFFSET(A24,1,0,1,1))</f>
-        <v>9</v>
+        <f ca="1">COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;A24)-COUNTIF(Gradebook!$AG$12:$AG$25,"&gt;="&amp;OFFSET(A24,1,0,1,1))</f>
+        <v>7</v>
       </c>
       <c r="D24" s="29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69230769230769229</v>
+        <v>0.53846153846153844</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
@@ -5471,8 +5672,8 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="54">
-        <f>Gradebook!$AF$26</f>
-        <v>0.93942122781065085</v>
+        <f>Gradebook!$AG$26</f>
+        <v>0.93226091177898418</v>
       </c>
       <c r="B28" s="55" t="str">
         <f>INDEX(B12:B24,MATCH(A28,A12:A24,1))</f>
@@ -5484,8 +5685,8 @@
         <v>49</v>
       </c>
       <c r="B30" s="54">
-        <f>Gradebook!AF27</f>
-        <v>0.96961538461538466</v>
+        <f>Gradebook!AG27</f>
+        <v>0.96160714285714288</v>
       </c>
       <c r="C30" s="63" t="s">
         <v>56</v>
@@ -5496,8 +5697,8 @@
         <v>50</v>
       </c>
       <c r="B31" s="54">
-        <f>Gradebook!AF28</f>
-        <v>7.7536248331331728E-2</v>
+        <f>Gradebook!AG28</f>
+        <v>7.4161714136325566E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
@@ -5697,8 +5898,8 @@
         <v>0.9</v>
       </c>
       <c r="B53" s="27">
-        <f>PERCENTILE(Gradebook!$AF$12:$AF$25,A53)</f>
-        <v>0.98590384615384619</v>
+        <f>PERCENTILE(Gradebook!$AG$12:$AG$25,A53)</f>
+        <v>0.98083333333333333</v>
       </c>
       <c r="C53" s="63" t="s">
         <v>62</v>
@@ -5711,8 +5912,8 @@
         <v>0.65</v>
       </c>
       <c r="B54" s="27">
-        <f>PERCENTILE(Gradebook!$AF$12:$AF$25,A54)</f>
-        <v>0.9789230769230769</v>
+        <f>PERCENTILE(Gradebook!$AG$12:$AG$25,A54)</f>
+        <v>0.97065476190476185</v>
       </c>
       <c r="D54" s="28"/>
       <c r="E54" s="28"/>
@@ -5722,8 +5923,8 @@
         <v>0.35</v>
       </c>
       <c r="B55" s="27">
-        <f>PERCENTILE(Gradebook!$AF$12:$AF$25,A55)</f>
-        <v>0.96430769230769231</v>
+        <f>PERCENTILE(Gradebook!$AG$12:$AG$25,A55)</f>
+        <v>0.93791666666666662</v>
       </c>
       <c r="D55" s="28"/>
       <c r="E55" s="28"/>
@@ -5733,8 +5934,8 @@
         <v>0.1</v>
       </c>
       <c r="B56" s="27">
-        <f>PERCENTILE(Gradebook!$AF$12:$AF$25,A56)</f>
-        <v>0.88276923076923075</v>
+        <f>PERCENTILE(Gradebook!$AG$12:$AG$25,A56)</f>
+        <v>0.86696428571428574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>